<commit_message>
v3 del comparador, con pasaporte en coreano
</commit_message>
<xml_diff>
--- a/01 (1).xlsx
+++ b/01 (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr updateLinks="never" codeName="현재_통합_문서" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\pyAlhambra\pyAlhambra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3991B2FA-3010-4F6D-A45C-5A49BE306161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBD3FFA-3607-4CAE-BD67-A8B01891B6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38304" yWindow="3852" windowWidth="14592" windowHeight="15576" tabRatio="775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="루밍" sheetId="25" r:id="rId1"/>
@@ -21,12 +21,12 @@
     <definedName name="시작요일">WEEKDAY(#REF!)</definedName>
     <definedName name="위치">(ROW()-4)*7+COLUMN()</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="289">
   <si>
     <t>상품명</t>
   </si>
@@ -986,6 +986,9 @@
   <si>
     <t>GUIA COREANO</t>
   </si>
+  <si>
+    <t>LIM KYUNG RAN1</t>
+  </si>
 </sst>
 </file>
 
@@ -993,11 +996,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="mmm/yy;@"/>
-    <numFmt numFmtId="179" formatCode="d/mmm;@"/>
-    <numFmt numFmtId="184" formatCode="&quot;ROOMING LIST &lt;&lt;&quot;@&quot;&gt;&gt;&quot;"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="mmm/yy;@"/>
+    <numFmt numFmtId="167" formatCode="d/mmm;@"/>
+    <numFmt numFmtId="168" formatCode="&quot;ROOMING LIST &lt;&lt;&quot;@&quot;&gt;&gt;&quot;"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1377,14 +1380,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -1479,10 +1482,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="179" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1536,7 +1539,7 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="20" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="20" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1934,28 +1937,28 @@
   <dimension ref="A1:BB48"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L55" sqref="A55:L56"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="19" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="20" customWidth="1"/>
-    <col min="6" max="7" width="10.140625" style="21" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="22" customWidth="1"/>
-    <col min="9" max="11" width="10.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="72.7109375" style="1" customWidth="1"/>
-    <col min="13" max="14" width="11.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" style="20" customWidth="1"/>
+    <col min="6" max="7" width="10.109375" style="21" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" style="22" customWidth="1"/>
+    <col min="9" max="11" width="10.6640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="72.6640625" style="1" customWidth="1"/>
+    <col min="13" max="14" width="11.6640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="13" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="1" customWidth="1"/>
-    <col min="17" max="49" width="3.42578125" style="30" customWidth="1"/>
-    <col min="50" max="50" width="3.42578125" style="31" customWidth="1"/>
-    <col min="51" max="51" width="3.42578125" style="30" customWidth="1"/>
-    <col min="52" max="52" width="3.42578125" style="31" customWidth="1"/>
-    <col min="53" max="54" width="3.42578125" style="30" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="1" customWidth="1"/>
+    <col min="17" max="49" width="3.44140625" style="30" customWidth="1"/>
+    <col min="50" max="50" width="3.44140625" style="31" customWidth="1"/>
+    <col min="51" max="51" width="3.44140625" style="30" customWidth="1"/>
+    <col min="52" max="52" width="3.44140625" style="31" customWidth="1"/>
+    <col min="53" max="54" width="3.44140625" style="30" customWidth="1"/>
     <col min="55" max="16384" width="10" style="2"/>
   </cols>
   <sheetData>
@@ -2122,7 +2125,7 @@
         <v>38</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>39</v>
+        <v>288</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>6</v>
@@ -2134,37 +2137,37 @@
         <v>187</v>
       </c>
       <c r="H6" s="13"/>
-      <c r="I6" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D6,$U$6:$U$500,0))</f>
-        <v>1972-02-06</v>
-      </c>
-      <c r="J6" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D6,$U$6:$U$500,0))</f>
-        <v>M719M6705</v>
-      </c>
-      <c r="K6" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D6,$U$6:$U$500,0))</f>
-        <v>2032-11-08</v>
-      </c>
-      <c r="L6" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D6,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
-        <v/>
-      </c>
-      <c r="M6" s="35" t="str">
+      <c r="I6" s="33" t="e">
+        <f t="shared" ref="I6:I47" si="0">INDEX($V$6:$V$500,MATCH(D6,$U$6:$U$500,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J6" s="33" t="e">
+        <f t="shared" ref="J6:J47" si="1">INDEX($Y$6:$Y$500,MATCH($D6,$U$6:$U$500,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K6" s="33" t="e">
+        <f t="shared" ref="K6:K47" si="2">INDEX($Z$6:$Z$500,MATCH($D6,$U$6:$U$500,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L6" s="34" t="e">
+        <f t="shared" ref="L6:L47" si="3">CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D6,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M6" s="35" t="e">
         <f>CLEAN(INDEX($AW$6:$AW$500,MATCH(D6,$AM$6:$AM$500,0)))</f>
-        <v/>
-      </c>
-      <c r="N6" s="35" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="N6" s="35" t="e">
         <f>CLEAN(INDEX($AX$6:$AX$500,MATCH(D6,$AM$6:$AM$500,0)))</f>
-        <v/>
-      </c>
-      <c r="O6" s="35" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O6" s="35" t="e">
         <f>CLEAN(INDEX($AY$6:$AY$500,MATCH(D6,$AM$6:$AM$500,0)))</f>
-        <v/>
-      </c>
-      <c r="P6" s="35" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="P6" s="35" t="e">
         <f>CLEAN(INDEX($AZ$6:$AZ$500,MATCH(D6,$AM$6:$AM$500,0)))</f>
-        <v/>
+        <v>#N/A</v>
       </c>
       <c r="Q6" s="30" t="s">
         <v>19</v>
@@ -2281,35 +2284,35 @@
       <c r="G7" s="14"/>
       <c r="H7" s="16"/>
       <c r="I7" s="37" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D7,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>2004-06-20</v>
       </c>
       <c r="J7" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D7,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M999F5270</v>
       </c>
       <c r="K7" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D7,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2032-11-28</v>
       </c>
       <c r="L7" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D7,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M7" s="35" t="str">
-        <f t="shared" ref="M7:M47" si="0">CLEAN(INDEX($AW$6:$AW$500,MATCH(D7,$AM$6:$AM$500,0)))</f>
+        <f t="shared" ref="M7:M47" si="4">CLEAN(INDEX($AW$6:$AW$500,MATCH(D7,$AM$6:$AM$500,0)))</f>
         <v/>
       </c>
       <c r="N7" s="35" t="str">
-        <f t="shared" ref="N7:N47" si="1">CLEAN(INDEX($AX$6:$AX$500,MATCH(D7,$AM$6:$AM$500,0)))</f>
+        <f t="shared" ref="N7:N47" si="5">CLEAN(INDEX($AX$6:$AX$500,MATCH(D7,$AM$6:$AM$500,0)))</f>
         <v/>
       </c>
       <c r="O7" s="35" t="str">
-        <f t="shared" ref="O7:O47" si="2">CLEAN(INDEX($AY$6:$AY$500,MATCH(D7,$AM$6:$AM$500,0)))</f>
+        <f t="shared" ref="O7:O47" si="6">CLEAN(INDEX($AY$6:$AY$500,MATCH(D7,$AM$6:$AM$500,0)))</f>
         <v/>
       </c>
       <c r="P7" s="35" t="str">
-        <f t="shared" ref="P7:P47" si="3">CLEAN(INDEX($AZ$6:$AZ$500,MATCH(D7,$AM$6:$AM$500,0)))</f>
+        <f t="shared" ref="P7:P47" si="7">CLEAN(INDEX($AZ$6:$AZ$500,MATCH(D7,$AM$6:$AM$500,0)))</f>
         <v/>
       </c>
       <c r="Q7" s="30" t="s">
@@ -2435,35 +2438,35 @@
         <v>128</v>
       </c>
       <c r="I8" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D8,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1970-08-23</v>
       </c>
       <c r="J8" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D8,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M479U9274</v>
       </c>
       <c r="K8" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D8,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2034-02-21</v>
       </c>
       <c r="L8" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D8,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>3#[하나팩2.0]GRX연장45.00/</v>
       </c>
       <c r="M8" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N8" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O8" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P8" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>ㄴ 계약금/리컨펌OK(8/7)</v>
       </c>
       <c r="AE8" s="30" t="s">
@@ -2548,35 +2551,35 @@
       <c r="G9" s="14"/>
       <c r="H9" s="16"/>
       <c r="I9" s="37" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D9,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>2000-11-30</v>
       </c>
       <c r="J9" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D9,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M69235406</v>
       </c>
       <c r="K9" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D9,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2029-05-29</v>
       </c>
       <c r="L9" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D9,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>3#[하나팩2.0]GRX연장45.00/</v>
       </c>
       <c r="M9" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N9" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O9" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P9" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AE9" s="30" t="s">
@@ -2664,35 +2667,35 @@
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D10,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1974-01-16</v>
       </c>
       <c r="J10" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D10,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M43077019</v>
       </c>
       <c r="K10" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D10,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2029-05-08</v>
       </c>
       <c r="L10" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D10,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M10" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N10" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>리컨펌OK</v>
       </c>
       <c r="O10" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>리컨펌ok11.29</v>
       </c>
       <c r="P10" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AE10" s="30" t="s">
@@ -2780,35 +2783,35 @@
       <c r="G11" s="14"/>
       <c r="H11" s="16"/>
       <c r="I11" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D11,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1973-03-12</v>
       </c>
       <c r="J11" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D11,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M85753242</v>
       </c>
       <c r="K11" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D11,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2028-02-28</v>
       </c>
       <c r="L11" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D11,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M11" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N11" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O11" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P11" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AE11" s="30" t="s">
@@ -2890,35 +2893,35 @@
       <c r="G12" s="14"/>
       <c r="H12" s="16"/>
       <c r="I12" s="36" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D12,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>2012-10-25</v>
       </c>
       <c r="J12" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D12,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M95769178</v>
       </c>
       <c r="K12" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D12,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2028-04-04</v>
       </c>
       <c r="L12" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D12,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M12" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N12" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O12" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P12" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AE12" s="30" t="s">
@@ -3006,35 +3009,35 @@
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D13,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1976-11-06</v>
       </c>
       <c r="J13" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D13,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M05714387</v>
       </c>
       <c r="K13" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D13,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2026-03-22</v>
       </c>
       <c r="L13" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D13,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>3#[하나팩2.0]GRX연장45.00/</v>
       </c>
       <c r="M13" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N13" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O13" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P13" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AE13" s="30" t="s">
@@ -3116,35 +3119,35 @@
       <c r="G14" s="14"/>
       <c r="H14" s="16"/>
       <c r="I14" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D14,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1975-08-28</v>
       </c>
       <c r="J14" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D14,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M452D5543</v>
       </c>
       <c r="K14" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D14,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2032-10-21</v>
       </c>
       <c r="L14" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D14,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>3#[하나팩2.0]GRX연장45.00/</v>
       </c>
       <c r="M14" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N14" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O14" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P14" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AE14" s="30" t="s">
@@ -3232,35 +3235,35 @@
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D15,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1974-01-08</v>
       </c>
       <c r="J15" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D15,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M58989087</v>
       </c>
       <c r="K15" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D15,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2028-10-29</v>
       </c>
       <c r="L15" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D15,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>싱글550,000/</v>
       </c>
       <c r="M15" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N15" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O15" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P15" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AE15" s="30" t="s">
@@ -3346,35 +3349,35 @@
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="36" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D16,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>2010-11-07</v>
       </c>
       <c r="J16" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D16,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M009L8437</v>
       </c>
       <c r="K16" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D16,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2029-11-01</v>
       </c>
       <c r="L16" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D16,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M16" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N16" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O16" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P16" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AE16" s="30" t="s">
@@ -3456,35 +3459,35 @@
       <c r="G17" s="14"/>
       <c r="H17" s="16"/>
       <c r="I17" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D17,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1976-05-22</v>
       </c>
       <c r="J17" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D17,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M699B1749</v>
       </c>
       <c r="K17" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D17,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2034-11-01</v>
       </c>
       <c r="L17" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D17,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M17" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N17" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O17" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P17" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AE17" s="30" t="s">
@@ -3572,35 +3575,35 @@
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D18,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1972-02-11</v>
       </c>
       <c r="J18" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D18,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M76566015</v>
       </c>
       <c r="K18" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D18,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2029-12-09</v>
       </c>
       <c r="L18" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D18,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M18" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N18" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O18" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>리컨펌ok11.28</v>
       </c>
       <c r="P18" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AE18" s="30" t="s">
@@ -3685,35 +3688,35 @@
       <c r="G19" s="14"/>
       <c r="H19" s="16"/>
       <c r="I19" s="36" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D19,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>2010-09-10</v>
       </c>
       <c r="J19" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D19,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M04205928</v>
       </c>
       <c r="K19" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D19,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2028-06-15</v>
       </c>
       <c r="L19" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D19,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M19" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N19" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O19" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P19" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AE19" s="30" t="s">
@@ -3801,35 +3804,35 @@
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D20,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1963-02-07</v>
       </c>
       <c r="J20" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D20,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M900P8714</v>
       </c>
       <c r="K20" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D20,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2032-12-27</v>
       </c>
       <c r="L20" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D20,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M20" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N20" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>[네이버하나투어]  * 예약대표자에게 발송드립니다.안녕하세요. 예약하신 상품의 상세 일정 및 포함 &amp; 불포함사항, 취소료 규정등 꼭 재확인 부탁드립니다.예약코드 : HP2422190566 (최예찬님외 1인 - 2인 1실 사용조건)상품명 : [출발확정] 스페인 일주 9일 #출발확정 #국적기직항 #시내호텔1박 #전일정4성호텔 #맛10 #플라멩고쇼 #몬세라트수도원 #루프탑레스토랑 #파라도르티타임 #세고비아 #론다출발일 : 2025-01-08 (수) 11:30 인천국제공항▶11월 29일 금요일까지 모든 여행자의 여권사본 및 만 18세 이상 연락처를 메일(hg665@hanatour.com) 로 발송해주세요. (여행지, 출발일 기재 필수)- 만료일이 지났거나 출발일기준 6개월 미만인경우 구여권 먼저 발송후 여권 재발급후 신규 여권사본 발송해주세요.- 신규발급예정인경우 - 여권 영문명 / 성별 / 법정생년월일 메일로 발송후 여권 발급 사본 발송해주세요.- 여권에 낙서가 있거나 훼손이 되었을 경우 출국이 안될 수 있습니다.2. 여행경비 잔금 결제 출발 한달전 네이버 페이 결제 링크 문자 발송으로 요청드립니다.[★모바일 일정표 꼭!! 확인해주세요★]https://www.hanatour.com/trp/pkg/CHPC0PKG0200M200?pkgCd=ESP131250108TWW&amp;type=H01[★참고사항 ★]네이버 결제상품으로 하나투어 예약조회 또는 카톡 계약서 동의 작성시 결제 요청은 미진행해주시면 됩니다. 감사합니다.  문의 사항 있으시면 연락 부탁드립니다. - 영업시간:평일 09:00~17:00 - 주말 및 공휴일, 점심시간(12시~13시) 통화불가담당자/이승희(본문자는 회신이 불가합니다.)</v>
       </c>
       <c r="O20" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>리컨펌ok1206</v>
       </c>
       <c r="P20" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>리컨펌OK / 제휴사결제 OK</v>
       </c>
       <c r="Q20" s="30" t="s">
@@ -3953,35 +3956,35 @@
       <c r="G21" s="14"/>
       <c r="H21" s="16"/>
       <c r="I21" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D21,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1964-11-06</v>
       </c>
       <c r="J21" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D21,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M72469216</v>
       </c>
       <c r="K21" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D21,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2026-03-02</v>
       </c>
       <c r="L21" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D21,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M21" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N21" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O21" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P21" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q21" s="30" t="s">
@@ -4102,35 +4105,35 @@
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D22,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1994-01-01</v>
       </c>
       <c r="J22" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D22,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M612R7682</v>
       </c>
       <c r="K22" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D22,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2034-06-13</v>
       </c>
       <c r="L22" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D22,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M22" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N22" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O22" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>리컨펌ok12.03</v>
       </c>
       <c r="P22" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>API연동/결제완료11343308531134420233스페인 일주 9일 #국적기직항 #시내호텔1박 #전일정4성호텔 #맛10 #플라멩고쇼 #론다 ＃코르도바 ＃세고비아★리컨펌OK</v>
       </c>
       <c r="Q22" s="30" t="s">
@@ -4253,35 +4256,35 @@
         <v>133</v>
       </c>
       <c r="I23" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D23,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1989-11-20</v>
       </c>
       <c r="J23" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D23,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M886G1545</v>
       </c>
       <c r="K23" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D23,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2032-04-07</v>
       </c>
       <c r="L23" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D23,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M23" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N23" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O23" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P23" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>[현대이지웰 하나투어]1월8일(수) 인천출발 스페인 일주 9일 여행상품 예약 안내 드립니다.해당 상품 출발 가능합니다.일정표(상세 일정 및 포함, 불포함 내역) 재확인 부탁드리며 진행 원하실경우 12월3일(화) 오전11시 전까지 결제(차액) 및 여권사본 전송 부탁 드립니다.취소마감일이 지난 예약으로 미결제시 취소되며 확정 후 취소 시 약관상 취소료가 부과됩니다.특별약관 적용 상품으로 취소 시 표준약관보다 높은 취소수수료가 부과됩니다. ※일정 및 호텔은 예정으로 출발 2~3일전 확정일정표에서 확인 가능합니다.★일정표 바로가기https://www.hanatour.com/trp/pkg/CHPC0PKG0200M200?pkgCd=ESP131250108TWW&amp;type=H01(위 링크 클릭시 상세일정 확인 가능합니다.)※해당 여행상품은 선택관광 등 추가 비용이 발생됩니다. 하나투어 일정표 꼭 재 확인 부탁 드립니다. ★여행경비 결제 안내 드립니다. 복지몰 홈페이지 -&gt; 여행레저 -&gt; 해외패키지 -&gt; 검색란 위에 '예약내역' -&gt;하단 '미결제금 결제하기'  에서 결제 완납 부탁 드립니다.(유류할증료에 따라 환불 또는 추가 결제 요청 드릴 수 있습니다.) &lt;여권사본 요청&gt;*메일 전송시: mjkim519@hanatour.com 으로 보내주세요.*문자 전송시: #12331000 으로 보내주세요.(#기호 꼭 넣어주세요.)(#1233-1000 번은  하나투어 수신전용 공식 MMS 번호입다. 보내신 정보는 개인정보보호법에 의거 접수 후 즉시 삭제됩니다.)문의사항 있으시면 연락주세요.감사합니다.▶ 하나투어 ☎ 02)2637-6891- 업무시간:평일 09:00~18:00- 주말 및 공휴일, 점심시간(12시~13시) 통화불가</v>
       </c>
       <c r="Q23" s="30" t="s">
@@ -4408,35 +4411,35 @@
       </c>
       <c r="H24" s="16"/>
       <c r="I24" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D24,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1965-06-16</v>
       </c>
       <c r="J24" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D24,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M18181454</v>
       </c>
       <c r="K24" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D24,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2029-12-16</v>
       </c>
       <c r="L24" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D24,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M24" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N24" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O24" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P24" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q24" s="30" t="s">
@@ -4558,35 +4561,35 @@
       <c r="G25" s="14"/>
       <c r="H25" s="16"/>
       <c r="I25" s="37" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D25,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>2006-03-30</v>
       </c>
       <c r="J25" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D25,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M096L3559</v>
       </c>
       <c r="K25" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D25,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2029-12-03</v>
       </c>
       <c r="L25" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D25,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M25" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N25" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O25" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P25" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q25" s="30" t="s">
@@ -4701,35 +4704,35 @@
       <c r="G26" s="14"/>
       <c r="H26" s="16"/>
       <c r="I26" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D26,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1962-10-09</v>
       </c>
       <c r="J26" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D26,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M89659894</v>
       </c>
       <c r="K26" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D26,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2029-12-20</v>
       </c>
       <c r="L26" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D26,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M26" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N26" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O26" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P26" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q26" s="30" t="s">
@@ -4851,35 +4854,35 @@
       </c>
       <c r="H27" s="16"/>
       <c r="I27" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D27,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1970-02-22</v>
       </c>
       <c r="J27" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D27,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M60830548</v>
       </c>
       <c r="K27" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D27,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2027-05-02</v>
       </c>
       <c r="L27" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D27,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M27" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N27" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O27" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P27" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q27" s="30" t="s">
@@ -4995,35 +4998,35 @@
       <c r="G28" s="14"/>
       <c r="H28" s="16"/>
       <c r="I28" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D28,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1966-01-11</v>
       </c>
       <c r="J28" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D28,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M75806443</v>
       </c>
       <c r="K28" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D28,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2026-02-16</v>
       </c>
       <c r="L28" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D28,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M28" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N28" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O28" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P28" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q28" s="30" t="s">
@@ -5145,35 +5148,35 @@
       </c>
       <c r="H29" s="16"/>
       <c r="I29" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D29,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1980-12-22</v>
       </c>
       <c r="J29" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D29,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M554D0735</v>
       </c>
       <c r="K29" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D29,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2033-11-15</v>
       </c>
       <c r="L29" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D29,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M29" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N29" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O29" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P29" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>리컨펌OK(10/14)</v>
       </c>
       <c r="AE29" s="30" t="s">
@@ -5255,35 +5258,35 @@
       <c r="G30" s="14"/>
       <c r="H30" s="16"/>
       <c r="I30" s="36" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D30,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>2012-06-11</v>
       </c>
       <c r="J30" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D30,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M387T0568</v>
       </c>
       <c r="K30" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D30,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2028-11-15</v>
       </c>
       <c r="L30" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D30,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M30" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N30" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O30" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P30" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q30" s="30" t="s">
@@ -5402,35 +5405,35 @@
       </c>
       <c r="H31" s="16"/>
       <c r="I31" s="36" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D31,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>2015-04-02</v>
       </c>
       <c r="J31" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D31,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M155D1284</v>
       </c>
       <c r="K31" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D31,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2028-11-15</v>
       </c>
       <c r="L31" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D31,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M31" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N31" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O31" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P31" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q31" s="30" t="s">
@@ -5545,35 +5548,35 @@
       <c r="G32" s="14"/>
       <c r="H32" s="16"/>
       <c r="I32" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D32,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1977-10-11</v>
       </c>
       <c r="J32" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D32,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M324J0594</v>
       </c>
       <c r="K32" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D32,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2033-11-27</v>
       </c>
       <c r="L32" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D32,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M32" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N32" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O32" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P32" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q32" s="30" t="s">
@@ -5700,35 +5703,35 @@
       </c>
       <c r="H33" s="16"/>
       <c r="I33" s="37" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D33,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>2006-10-17</v>
       </c>
       <c r="J33" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D33,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M93989361</v>
       </c>
       <c r="K33" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D33,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2028-02-03</v>
       </c>
       <c r="L33" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D33,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>싱글550,000/</v>
       </c>
       <c r="M33" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N33" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O33" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P33" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q33" s="30" t="s">
@@ -5851,35 +5854,35 @@
       </c>
       <c r="H34" s="16"/>
       <c r="I34" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D34,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1976-06-22</v>
       </c>
       <c r="J34" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D34,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M752P8539</v>
       </c>
       <c r="K34" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D34,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2034-12-05</v>
       </c>
       <c r="L34" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D34,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M34" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N34" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O34" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P34" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">리컨펌OK - 1216수험생1+동반자1 각각 10만원씩 할인 적용OKㄴ2~3번 고객 </v>
       </c>
       <c r="Q34" s="30" t="s">
@@ -5997,35 +6000,35 @@
       <c r="G35" s="14"/>
       <c r="H35" s="16"/>
       <c r="I35" s="33" t="str">
-        <f>INDEX($V$6:$V$500,MATCH(D35,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>1975-04-24</v>
       </c>
       <c r="J35" s="33" t="str">
-        <f>INDEX($Y$6:$Y$500,MATCH($D35,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>M986C8950</v>
       </c>
       <c r="K35" s="33" t="str">
-        <f>INDEX($Z$6:$Z$500,MATCH($D35,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>2034-04-30</v>
       </c>
       <c r="L35" s="34" t="str">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D35,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M35" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N35" s="35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O35" s="35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P35" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q35" s="30" t="s">
@@ -6142,35 +6145,35 @@
       </c>
       <c r="H36" s="16"/>
       <c r="I36" s="33" t="e">
-        <f>INDEX($V$6:$V$500,MATCH(D36,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="J36" s="33" t="e">
-        <f>INDEX($Y$6:$Y$500,MATCH($D36,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="K36" s="33" t="e">
-        <f>INDEX($Z$6:$Z$500,MATCH($D36,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="L36" s="34" t="e">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D36,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="M36" s="35" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="N36" s="35" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
       <c r="O36" s="35" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="P36" s="35" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="Q36" s="30" t="s">
@@ -6219,35 +6222,35 @@
       <c r="G37" s="14"/>
       <c r="H37" s="16"/>
       <c r="I37" s="33" t="e">
-        <f>INDEX($V$6:$V$500,MATCH(D37,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="J37" s="33" t="e">
-        <f>INDEX($Y$6:$Y$500,MATCH($D37,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="K37" s="33" t="e">
-        <f>INDEX($Z$6:$Z$500,MATCH($D37,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="L37" s="34" t="e">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D37,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="M37" s="35" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="N37" s="35" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
       <c r="O37" s="35" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="P37" s="35" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="Q37" s="30" t="s">
@@ -6297,35 +6300,35 @@
       <c r="G38" s="14"/>
       <c r="H38" s="16"/>
       <c r="I38" s="33" t="e">
-        <f>INDEX($V$6:$V$500,MATCH(D38,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="J38" s="33" t="e">
-        <f>INDEX($Y$6:$Y$500,MATCH($D38,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="K38" s="33" t="e">
-        <f>INDEX($Z$6:$Z$500,MATCH($D38,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="L38" s="34" t="e">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D38,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="M38" s="35" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="N38" s="35" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
       <c r="O38" s="35" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="P38" s="35" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="Q38" s="30" t="s">
@@ -6375,35 +6378,35 @@
       <c r="G39" s="14"/>
       <c r="H39" s="16"/>
       <c r="I39" s="33" t="e">
-        <f>INDEX($V$6:$V$500,MATCH(D39,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="J39" s="33" t="e">
-        <f>INDEX($Y$6:$Y$500,MATCH($D39,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="K39" s="33" t="e">
-        <f>INDEX($Z$6:$Z$500,MATCH($D39,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="L39" s="34" t="e">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D39,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="M39" s="35" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="N39" s="35" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
       <c r="O39" s="35" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="P39" s="35" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="Q39" s="30" t="s">
@@ -6453,35 +6456,35 @@
       <c r="G40" s="14"/>
       <c r="H40" s="16"/>
       <c r="I40" s="33" t="e">
-        <f>INDEX($V$6:$V$500,MATCH(D40,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="J40" s="33" t="e">
-        <f>INDEX($Y$6:$Y$500,MATCH($D40,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="K40" s="33" t="e">
-        <f>INDEX($Z$6:$Z$500,MATCH($D40,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="L40" s="34" t="e">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D40,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="M40" s="35" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="N40" s="35" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
       <c r="O40" s="35" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="P40" s="35" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="Q40" s="30" t="s">
@@ -6528,35 +6531,35 @@
       <c r="G41" s="14"/>
       <c r="H41" s="16"/>
       <c r="I41" s="33" t="e">
-        <f>INDEX($V$6:$V$500,MATCH(D41,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="J41" s="33" t="e">
-        <f>INDEX($Y$6:$Y$500,MATCH($D41,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="K41" s="33" t="e">
-        <f>INDEX($Z$6:$Z$500,MATCH($D41,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="L41" s="34" t="e">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D41,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="M41" s="35" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="N41" s="35" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
       <c r="O41" s="35" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="P41" s="35" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="Q41" s="30" t="s">
@@ -6603,35 +6606,35 @@
       <c r="G42" s="14"/>
       <c r="H42" s="16"/>
       <c r="I42" s="33" t="e">
-        <f>INDEX($V$6:$V$500,MATCH(D42,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="J42" s="33" t="e">
-        <f>INDEX($Y$6:$Y$500,MATCH($D42,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="K42" s="33" t="e">
-        <f>INDEX($Z$6:$Z$500,MATCH($D42,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="L42" s="34" t="e">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D42,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="M42" s="35" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="N42" s="35" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
       <c r="O42" s="35" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="P42" s="35" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="Q42" s="30" t="s">
@@ -6678,35 +6681,35 @@
       <c r="G43" s="14"/>
       <c r="H43" s="16"/>
       <c r="I43" s="33" t="e">
-        <f>INDEX($V$6:$V$500,MATCH(D43,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="J43" s="33" t="e">
-        <f>INDEX($Y$6:$Y$500,MATCH($D43,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="K43" s="33" t="e">
-        <f>INDEX($Z$6:$Z$500,MATCH($D43,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="L43" s="34" t="e">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D43,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="M43" s="35" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="N43" s="35" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
       <c r="O43" s="35" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="P43" s="35" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="Q43" s="30" t="s">
@@ -6753,35 +6756,35 @@
       <c r="G44" s="14"/>
       <c r="H44" s="16"/>
       <c r="I44" s="33" t="e">
-        <f>INDEX($V$6:$V$500,MATCH(D44,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="J44" s="33" t="e">
-        <f>INDEX($Y$6:$Y$500,MATCH($D44,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="K44" s="33" t="e">
-        <f>INDEX($Z$6:$Z$500,MATCH($D44,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="L44" s="34" t="e">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D44,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="M44" s="35" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="N44" s="35" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
       <c r="O44" s="35" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="P44" s="35" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="Q44" s="30" t="s">
@@ -6834,35 +6837,35 @@
       <c r="G45" s="14"/>
       <c r="H45" s="16"/>
       <c r="I45" s="33" t="e">
-        <f>INDEX($V$6:$V$500,MATCH(D45,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="J45" s="33" t="e">
-        <f>INDEX($Y$6:$Y$500,MATCH($D45,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="K45" s="33" t="e">
-        <f>INDEX($Z$6:$Z$500,MATCH($D45,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="L45" s="34" t="e">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D45,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="M45" s="35" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="N45" s="35" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
       <c r="O45" s="35" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="P45" s="35" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="Q45" s="30" t="s">
@@ -6915,35 +6918,35 @@
       <c r="G46" s="14"/>
       <c r="H46" s="16"/>
       <c r="I46" s="33" t="e">
-        <f>INDEX($V$6:$V$500,MATCH(D46,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="J46" s="33" t="e">
-        <f>INDEX($Y$6:$Y$500,MATCH($D46,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="K46" s="33" t="e">
-        <f>INDEX($Z$6:$Z$500,MATCH($D46,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="L46" s="34" t="e">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D46,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="M46" s="35" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="N46" s="35" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
       <c r="O46" s="35" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="P46" s="35" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="Q46" s="30" t="s">
@@ -6990,35 +6993,35 @@
       <c r="G47" s="17"/>
       <c r="H47" s="16"/>
       <c r="I47" s="33" t="e">
-        <f>INDEX($V$6:$V$500,MATCH(D47,$U$6:$U$500,0))</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="J47" s="33" t="e">
-        <f>INDEX($Y$6:$Y$500,MATCH($D47,$U$6:$U$500,0))</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="K47" s="33" t="e">
-        <f>INDEX($Z$6:$Z$500,MATCH($D47,$U$6:$U$500,0))</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="L47" s="34" t="e">
-        <f>CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D47,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="M47" s="35" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
       <c r="N47" s="35" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
       <c r="O47" s="35" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="P47" s="35" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="Q47" s="30" t="s">
@@ -7105,7 +7108,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.37" right="0.2" top="1.07" bottom="0.17" header="0.28999999999999998" footer="0.22"/>
-  <pageSetup paperSize="9" scale="87" fitToWidth="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="85" fitToWidth="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"+,보통"&amp;10&amp;G
 46/50 COOMBE ROAD, NEWMALDEN, SURREY, KT3 4QF, UNITED KINGDOM 

</xml_diff>